<commit_message>
apex TCDS links work
</commit_message>
<xml_diff>
--- a/examples/apex_USp/src/link_map_apex_ku15p_gth.xlsx
+++ b/examples/apex_USp/src/link_map_apex_ku15p_gth.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="36">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -61,16 +61,13 @@
     <t xml:space="preserve">index</t>
   </si>
   <si>
-    <t xml:space="preserve">real Y</t>
-  </si>
-  <si>
     <t xml:space="preserve">rx</t>
   </si>
   <si>
     <t xml:space="preserve">0</t>
   </si>
   <si>
-    <t xml:space="preserve">28</t>
+    <t xml:space="preserve">32</t>
   </si>
   <si>
     <t xml:space="preserve">TCDS</t>
@@ -85,22 +82,46 @@
     <t xml:space="preserve">tcds_rx</t>
   </si>
   <si>
-    <t xml:space="preserve">29</t>
+    <t xml:space="preserve">33</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">30</t>
+    <t xml:space="preserve">34</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">31</t>
+    <t xml:space="preserve">35</t>
   </si>
   <si>
     <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
   </si>
   <si>
     <t xml:space="preserve">tx</t>
@@ -227,10 +248,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -305,225 +326,423 @@
       <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="2" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="D17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="3" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="D18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>